<commit_message>
Monday motivation || Restartured QuizApp excel sheet
</commit_message>
<xml_diff>
--- a/App_Data/QuizApplication.xlsx
+++ b/App_Data/QuizApplication.xlsx
@@ -3,19 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD7B907-F813-44F3-898A-5488D10BF0B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA9346E-71F7-40C9-86CE-57E8B9A8D022}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1210" yWindow="-110" windowWidth="18100" windowHeight="11020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="-108" windowWidth="22128" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="To Do List - POC" sheetId="7" r:id="rId1"/>
-    <sheet name="Questions" sheetId="8" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="10" r:id="rId3"/>
-    <sheet name="Assignment Setup" sheetId="6" r:id="rId4"/>
-    <sheet name="To Do List-RoadMap" sheetId="9" r:id="rId5"/>
+    <sheet name="To Do List" sheetId="7" r:id="rId1"/>
+    <sheet name="To Do - Details" sheetId="8" r:id="rId2"/>
+    <sheet name="FunApp-RoadMap" sheetId="9" r:id="rId3"/>
+    <sheet name="2021_WorkProgress" sheetId="11" r:id="rId4"/>
+    <sheet name="Assignment Setup" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="Assignedto" localSheetId="4">ColorKeys[Assigned To]</definedName>
+    <definedName name="Assignedto" localSheetId="3">ColorKeys[Assigned To]</definedName>
+    <definedName name="Assignedto" localSheetId="2">ColorKeys[Assigned To]</definedName>
     <definedName name="Assignedto">ColorKeys[Assigned To]</definedName>
     <definedName name="Color1">'Assignment Setup'!$B$4</definedName>
     <definedName name="Color2">'Assignment Setup'!$B$5</definedName>
@@ -23,18 +24,24 @@
     <definedName name="Color4">'Assignment Setup'!$B$7</definedName>
     <definedName name="Color5">'Assignment Setup'!$B$8</definedName>
     <definedName name="Color6">'Assignment Setup'!$B$9</definedName>
-    <definedName name="ColorKey" localSheetId="4">ColorKeys[Assigned To]</definedName>
+    <definedName name="ColorKey" localSheetId="3">ColorKeys[Assigned To]</definedName>
+    <definedName name="ColorKey" localSheetId="2">ColorKeys[Assigned To]</definedName>
     <definedName name="ColorKey">ColorKeys[Assigned To]</definedName>
-    <definedName name="ColumnTitle1" localSheetId="4">ToDoList2[[#Headers],[Done]]</definedName>
+    <definedName name="ColumnTitle1" localSheetId="3">ToDoList4[[#Headers],[Done]]</definedName>
+    <definedName name="ColumnTitle1" localSheetId="2">ToDoList2[[#Headers],[Done]]</definedName>
     <definedName name="ColumnTitle1">ToDoList[[#Headers],[Done]]</definedName>
-    <definedName name="ColumnTitle2" localSheetId="4">ColorKeys[[#Headers],[Assigned To]]</definedName>
+    <definedName name="ColumnTitle2" localSheetId="3">ColorKeys[[#Headers],[Assigned To]]</definedName>
+    <definedName name="ColumnTitle2" localSheetId="2">ColorKeys[[#Headers],[Assigned To]]</definedName>
     <definedName name="ColumnTitle2">ColorKeys[[#Headers],[Assigned To]]</definedName>
-    <definedName name="DueToday" localSheetId="4">'To Do List-RoadMap'!$C$3</definedName>
-    <definedName name="DueToday">'To Do List - POC'!$C$3</definedName>
+    <definedName name="DueToday" localSheetId="3">'2021_WorkProgress'!$C$3</definedName>
+    <definedName name="DueToday" localSheetId="2">'FunApp-RoadMap'!$C$3</definedName>
+    <definedName name="DueToday">'To Do List'!$C$3</definedName>
+    <definedName name="Grid" localSheetId="3">ToDoList4[[#All],[Description]:[Assigned to]]</definedName>
+    <definedName name="Grid" localSheetId="2">ToDoList2[[#All],[Description]:[Assigned to]]</definedName>
     <definedName name="Grid" localSheetId="0">ToDoList[[#All],[Description]:[Assigned to]]</definedName>
-    <definedName name="Grid" localSheetId="4">ToDoList2[[#All],[Description]:[Assigned to]]</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'To Do List - POC'!$1:$6</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="4">'To Do List-RoadMap'!$1:$6</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="3">'2021_WorkProgress'!$1:$6</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="2">'FunApp-RoadMap'!$1:$6</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'To Do List'!$1:$6</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -52,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="109">
   <si>
     <t xml:space="preserve">                            </t>
   </si>
@@ -200,9 +207,6 @@
     <t>Panda</t>
   </si>
   <si>
-    <t xml:space="preserve">Technical Expert </t>
-  </si>
-  <si>
     <t xml:space="preserve">Developer </t>
   </si>
   <si>
@@ -358,9 +362,6 @@
     <t>7.Hint Section on the top: Disappear the two answer list</t>
   </si>
   <si>
-    <t>--------------------</t>
-  </si>
-  <si>
     <t>https://github.com/mattboldt/typed.js/issues/396</t>
   </si>
   <si>
@@ -368,6 +369,57 @@
   </si>
   <si>
     <t>ToDo</t>
+  </si>
+  <si>
+    <t>Display who answered first on submit</t>
+  </si>
+  <si>
+    <t>Server response using Signal R</t>
+  </si>
+  <si>
+    <t>Rajish and Asish</t>
+  </si>
+  <si>
+    <t>Admin Page Display (CRUD)</t>
+  </si>
+  <si>
+    <t>Defect Fix (Please look into To-Do Details)</t>
+  </si>
+  <si>
+    <t>From Raghu?</t>
+  </si>
+  <si>
+    <t>Infrastructure</t>
+  </si>
+  <si>
+    <t>1. Web Server where we can host website</t>
+  </si>
+  <si>
+    <t>2. SQL DataBase to Deploy the DB</t>
+  </si>
+  <si>
+    <t>Future:</t>
+  </si>
+  <si>
+    <t>Enable the url without VPN with token</t>
+  </si>
+  <si>
+    <t>Android App using DotNet</t>
+  </si>
+  <si>
+    <t>Steps to add Questions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. Add the QuestionGroup Name in Quiz table</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2. Add a question in Questions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3. Add the AnswerChoices in  the [Choices] table with the corresponding question identity value</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4. Add a record for Answers in the Answers Table</t>
   </si>
 </sst>
 </file>
@@ -381,7 +433,7 @@
     <numFmt numFmtId="167" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
     <numFmt numFmtId="168" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.14996795556505021"/>
@@ -602,6 +654,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF262626"/>
+      <name val="Lucida Sans"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -635,7 +694,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -672,6 +731,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFC8F0FF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="6" tint="0.79998168889431442"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1">
@@ -691,7 +768,7 @@
     <xf numFmtId="167" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="14" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -828,6 +905,21 @@
     <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="20% - Accent5" xfId="1" builtinId="46"/>
@@ -843,7 +935,58 @@
     <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="8" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="85">
+  <dxfs count="136">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <u val="none"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="6" tint="0.79998168889431442"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <name val="Rockwell"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -942,6 +1085,11 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <color auto="1"/>
       </font>
     </dxf>
@@ -972,11 +1120,6 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="3"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <color auto="1"/>
       </font>
     </dxf>
@@ -1042,15 +1185,150 @@
     </dxf>
     <dxf>
       <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <u val="none"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <u val="none"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <u val="none"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="3"/>
       </font>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="6" tint="0.79998168889431442"/>
-        </bottom>
-      </border>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <u val="none"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="&quot;Done&quot;;&quot;&quot;;&quot;&quot;"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1059,11 +1337,181 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="0"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.14996795556505021"/>
         <name val="Rockwell"/>
         <family val="1"/>
         <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <u val="none"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <u val="none"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <u val="none"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <u val="none"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <u val="none"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
       </font>
     </dxf>
     <dxf>
@@ -1478,14 +1926,14 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="To Do List" defaultPivotStyle="PivotStyleLight18">
     <tableStyle name="Address Book" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="84"/>
-      <tableStyleElement type="headerRow" dxfId="83"/>
-      <tableStyleElement type="firstRowStripe" dxfId="82"/>
-      <tableStyleElement type="secondRowStripe" dxfId="81"/>
+      <tableStyleElement type="wholeTable" dxfId="135"/>
+      <tableStyleElement type="headerRow" dxfId="134"/>
+      <tableStyleElement type="firstRowStripe" dxfId="133"/>
+      <tableStyleElement type="secondRowStripe" dxfId="132"/>
     </tableStyle>
     <tableStyle name="To Do List" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="80"/>
-      <tableStyleElement type="headerRow" dxfId="79"/>
+      <tableStyleElement type="wholeTable" dxfId="131"/>
+      <tableStyleElement type="headerRow" dxfId="130"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -2130,15 +2578,327 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>990600</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>21600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Data Entry Tip" descr="Enter a number greater than 1 in Done column when  task is complete">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5020EA12-0F30-4F68-8E17-BAB8C6D2EE1F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3406140" y="1112520"/>
+          <a:ext cx="990600" cy="600720"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="72000" tIns="0" rIns="72000" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="800">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Enter a number 1 in Done column when  task is complete</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData fPrintsWithSheet="0"/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>21600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Data Entry Tip" descr="Enter a number greater than 1 in Done column when  task is complete">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B016A975-C429-4676-9694-847F614094F9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4434840" y="1112520"/>
+          <a:ext cx="2194560" cy="600720"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="72000" tIns="0" rIns="72000" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="800">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Select</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="800" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> a drop down arrow, such as </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="800">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Assigned To or Priority,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="800" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="800">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>to Filter or Sort your To Do List items.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="800">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="800">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>T</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="800" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>ips </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="800">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>do not print.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="800">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData fPrintsWithSheet="0"/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>177512</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>111667</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>626669</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>762687</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="Decorative element&#10;">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D70D7AAB-B1E3-4AF3-B349-26858E2CF24B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm rot="21012350">
+          <a:off x="329912" y="111667"/>
+          <a:ext cx="449157" cy="651020"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ToDoList" displayName="ToDoList" ref="B6:F17" totalsRowShown="0" headerRowDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ToDoList" displayName="ToDoList" ref="B6:F17" totalsRowShown="0" headerRowDxfId="88">
   <autoFilter ref="B6:F17" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Done" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Description" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Due Date" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Priority" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Assigned to" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Done" dataDxfId="87"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Description" dataDxfId="86"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Due Date" dataDxfId="85"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Priority" dataDxfId="84"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Assigned to" dataDxfId="83"/>
   </tableColumns>
   <tableStyleInfo name="Address Book" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2150,7 +2910,45 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="ColorKeys" displayName="ColorKeys" ref="B3:C9" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EAB70A46-0CF0-4D35-9438-FC09BD356BF6}" name="ToDoList2" displayName="ToDoList2" ref="B6:F13" totalsRowShown="0" headerRowDxfId="58">
+  <autoFilter ref="B6:F13" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{6D55EE3E-E775-41B3-BC0A-08AC46F6EF17}" name="Done" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{A568071C-C7BC-49A3-A2AE-BC0A89D3D4A4}" name="Description" dataDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{BE941CF0-BB93-4A44-A031-79654E12770C}" name="Due Date" dataDxfId="55"/>
+    <tableColumn id="4" xr3:uid="{198586D7-EC80-4B60-A7EF-306798680CD2}" name="Priority" dataDxfId="54"/>
+    <tableColumn id="5" xr3:uid="{ECB977EA-E1B7-4EE3-9E79-1070BBA35C42}" name="Assigned to" dataDxfId="53"/>
+  </tableColumns>
+  <tableStyleInfo name="Address Book" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{504A1905-F514-4f6f-8877-14C23A59335A}">
+      <x14:table altTextSummary="Enter 1 to mark task as Done, Description, and Due Date, and select Priority and Assigned to names in this table"/>
+    </ext>
+  </extLst>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AE7EE83F-8E62-4BCF-B169-EBD3D0E85BEF}" name="ToDoList4" displayName="ToDoList4" ref="B6:F17" totalsRowShown="0" headerRowDxfId="11">
+  <autoFilter ref="B6:F17" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{6822DCC8-0392-486B-8480-4FB115516904}" name="Done" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{4942A3B4-C013-4609-95C7-B7BF88BDEE37}" name="Description" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{0C52536F-1EFF-49FC-8E87-5789F5F15AD5}" name="Due Date" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{7D2DCE90-A34A-4881-B20D-2D149D62374F}" name="Priority" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{D881DC46-F30D-426B-8535-304AF38351F1}" name="Assigned to" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="Address Book" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{504A1905-F514-4f6f-8877-14C23A59335A}">
+      <x14:table altTextSummary="Enter 1 to mark task as Done, Description, and Due Date, and select Priority and Assigned to names in this table"/>
+    </ext>
+  </extLst>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="ColorKeys" displayName="ColorKeys" ref="B3:C9" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4">
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Assigned To"/>
     <tableColumn id="2" xr3:uid="{F36E0378-7DB9-42F4-B4F4-263BE6500357}" name="Column1"/>
@@ -2159,25 +2957,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{504A1905-F514-4f6f-8877-14C23A59335A}">
       <x14:table altTextSummary="Insert or modify Assigned To names in this table"/>
-    </ext>
-  </extLst>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EAB70A46-0CF0-4D35-9438-FC09BD356BF6}" name="ToDoList2" displayName="ToDoList2" ref="B6:F13" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="B6:F13" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{6D55EE3E-E775-41B3-BC0A-08AC46F6EF17}" name="Done" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{A568071C-C7BC-49A3-A2AE-BC0A89D3D4A4}" name="Description" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{BE941CF0-BB93-4A44-A031-79654E12770C}" name="Due Date" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{198586D7-EC80-4B60-A7EF-306798680CD2}" name="Priority" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{ECB977EA-E1B7-4EE3-9E79-1070BBA35C42}" name="Assigned to" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="Address Book" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{504A1905-F514-4f6f-8877-14C23A59335A}">
-      <x14:table altTextSummary="Enter 1 to mark task as Done, Description, and Due Date, and select Priority and Assigned to names in this table"/>
     </ext>
   </extLst>
 </table>
@@ -2416,27 +3195,27 @@
   </sheetPr>
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.78515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="20.28515625" style="2" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" style="4" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="1.81640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="27.26953125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.7265625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="16.7265625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="18.54296875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="7.7265625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="20.26953125" style="2" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="17.26953125" style="4" hidden="1" customWidth="1"/>
     <col min="10" max="14" width="0" style="4" hidden="1" customWidth="1"/>
     <col min="15" max="17" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.7109375" style="2" hidden="1"/>
+    <col min="18" max="16384" width="10.7265625" style="2" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="66" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:17" ht="66" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -2459,11 +3238,11 @@
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
     </row>
-    <row r="2" spans="1:17" ht="21.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:17" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="12"/>
       <c r="B2" s="43">
         <f ca="1">TODAY()</f>
-        <v>44505</v>
+        <v>44598</v>
       </c>
       <c r="C2" s="43"/>
       <c r="D2" s="18"/>
@@ -2478,7 +3257,7 @@
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
     </row>
-    <row r="3" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="22" t="s">
         <v>9</v>
@@ -2499,7 +3278,7 @@
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
     </row>
-    <row r="4" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="22" t="s">
         <v>10</v>
@@ -2521,7 +3300,7 @@
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
     </row>
-    <row r="5" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="7"/>
       <c r="C5" s="14"/>
       <c r="D5" s="11"/>
@@ -2535,7 +3314,7 @@
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
     </row>
-    <row r="6" spans="1:17" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15"/>
       <c r="B6" s="24" t="s">
         <v>2</v>
@@ -2559,19 +3338,19 @@
       <c r="N6" s="15"/>
       <c r="O6" s="15"/>
     </row>
-    <row r="7" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="42" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>18</v>
+        <v>92</v>
       </c>
       <c r="D7" s="6">
-        <f ca="1">TODAY()-1</f>
-        <v>44504</v>
+        <f ca="1">TODAY()+11</f>
+        <v>44609</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>5</v>
@@ -2586,23 +3365,23 @@
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="42"/>
       <c r="B8" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>20</v>
+        <v>93</v>
       </c>
       <c r="D8" s="6">
-        <f ca="1">TODAY()+2</f>
-        <v>44507</v>
+        <f ca="1">TODAY()+15</f>
+        <v>44613</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -2611,23 +3390,23 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="42"/>
       <c r="B9" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
       <c r="D9" s="6">
-        <f ca="1">TODAY()+1</f>
-        <v>44506</v>
+        <f ca="1">TODAY()+20</f>
+        <v>44618</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -2636,23 +3415,23 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="42"/>
       <c r="B10" s="9">
         <v>0</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>42</v>
+        <v>96</v>
       </c>
       <c r="D10" s="6">
-        <f ca="1">TODAY()+1</f>
-        <v>44506</v>
+        <f ca="1">TODAY()+20</f>
+        <v>44618</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>26</v>
+        <v>94</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -2661,24 +3440,15 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="42"/>
       <c r="B11" s="9">
-        <v>1</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="6">
-        <f ca="1">TODAY()+2</f>
-        <v>44507</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>26</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -2686,23 +3456,14 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="9">
-        <v>1</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="6">
-        <f ca="1">TODAY()+8</f>
-        <v>44513</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -2710,23 +3471,14 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="32">
-        <v>1</v>
-      </c>
-      <c r="C13" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="34">
-        <f ca="1">TODAY()+5</f>
-        <v>44510</v>
-      </c>
-      <c r="E13" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="35" t="s">
-        <v>38</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C13" s="33"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -2734,21 +3486,12 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="9"/>
-      <c r="C14" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="6">
-        <f ca="1">TODAY()+2</f>
-        <v>44507</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -2756,21 +3499,12 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="9"/>
-      <c r="C15" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="6">
-        <f ca="1">TODAY()+2</f>
-        <v>44507</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -2778,21 +3512,12 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
     </row>
-    <row r="16" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="9"/>
-      <c r="C16" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="6">
-        <f ca="1">TODAY()+3</f>
-        <v>44508</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -2800,11 +3525,9 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="2:6" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="37"/>
-      <c r="C17" s="31" t="s">
-        <v>56</v>
-      </c>
+      <c r="C17" s="31"/>
       <c r="D17" s="38"/>
       <c r="E17" s="39"/>
       <c r="F17" s="39"/>
@@ -2815,153 +3538,153 @@
     <mergeCell ref="B2:C2"/>
   </mergeCells>
   <conditionalFormatting sqref="C7:C8 C14:C15 C11:C12">
-    <cfRule type="expression" dxfId="78" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="129" priority="45" stopIfTrue="1">
       <formula>D7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:F8 C14:F15 C11:F12">
-    <cfRule type="expression" dxfId="77" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="128" priority="43" stopIfTrue="1">
       <formula>$B7=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="44">
+    <cfRule type="expression" dxfId="127" priority="44">
       <formula>$D7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="46">
+    <cfRule type="expression" dxfId="126" priority="46">
       <formula>AND(B7&lt;&gt;1,D7=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="47">
+    <cfRule type="expression" dxfId="125" priority="47">
       <formula>AND($B7&lt;&gt;1,$D7&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="73" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="124" priority="30" stopIfTrue="1">
       <formula>D16=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16">
-    <cfRule type="expression" dxfId="72" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="123" priority="37" stopIfTrue="1">
       <formula>$B16=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="38">
+    <cfRule type="expression" dxfId="122" priority="38">
       <formula>$D16=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="40">
+    <cfRule type="expression" dxfId="121" priority="40">
       <formula>AND(E16&lt;&gt;1,G16=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="41">
+    <cfRule type="expression" dxfId="120" priority="41">
       <formula>AND($B16&lt;&gt;1,$D16&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16">
-    <cfRule type="expression" dxfId="68" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="119" priority="33" stopIfTrue="1">
       <formula>$B16=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="34">
+    <cfRule type="expression" dxfId="118" priority="34">
       <formula>$D16=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="35">
+    <cfRule type="expression" dxfId="117" priority="35">
       <formula>AND(C16&lt;&gt;1,E16=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="36">
+    <cfRule type="expression" dxfId="116" priority="36">
       <formula>AND($B16&lt;&gt;1,$D16&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="64" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="115" priority="28" stopIfTrue="1">
       <formula>$B16=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="29">
+    <cfRule type="expression" dxfId="114" priority="29">
       <formula>$D16=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="31">
+    <cfRule type="expression" dxfId="113" priority="31">
       <formula>AND(B16&lt;&gt;1,D16=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="32">
+    <cfRule type="expression" dxfId="112" priority="32">
       <formula>AND($B16&lt;&gt;1,$D16&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="expression" dxfId="60" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="111" priority="24" stopIfTrue="1">
       <formula>$B16=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="25">
+    <cfRule type="expression" dxfId="110" priority="25">
       <formula>$D16=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="26">
+    <cfRule type="expression" dxfId="109" priority="26">
       <formula>AND(D16&lt;&gt;1,F16=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="27">
+    <cfRule type="expression" dxfId="108" priority="27">
       <formula>AND($B16&lt;&gt;1,$D16&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="56" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="107" priority="20" stopIfTrue="1">
       <formula>D13=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13:F13">
-    <cfRule type="expression" dxfId="55" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="106" priority="18" stopIfTrue="1">
       <formula>$B13=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="19">
+    <cfRule type="expression" dxfId="105" priority="19">
       <formula>$D13=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="21">
+    <cfRule type="expression" dxfId="104" priority="21">
       <formula>AND(B13&lt;&gt;1,D13=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="22">
+    <cfRule type="expression" dxfId="103" priority="22">
       <formula>AND($B13&lt;&gt;1,$D13&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9:F9">
-    <cfRule type="expression" dxfId="51" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="12" stopIfTrue="1">
       <formula>$B9=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="13">
+    <cfRule type="expression" dxfId="101" priority="13">
       <formula>$D9=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="15">
+    <cfRule type="expression" dxfId="100" priority="15">
       <formula>AND(C9&lt;&gt;1,E9=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="16">
+    <cfRule type="expression" dxfId="99" priority="16">
       <formula>AND($B9&lt;&gt;1,$D9&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="47" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="98" priority="8" stopIfTrue="1">
       <formula>D10=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:F10">
-    <cfRule type="expression" dxfId="46" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="6" stopIfTrue="1">
       <formula>$B10=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="7">
+    <cfRule type="expression" dxfId="96" priority="7">
       <formula>$D10=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="9">
+    <cfRule type="expression" dxfId="95" priority="9">
       <formula>AND(B10&lt;&gt;1,D10=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="10">
+    <cfRule type="expression" dxfId="94" priority="10">
       <formula>AND($B10&lt;&gt;1,$D10&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="42" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="3" stopIfTrue="1">
       <formula>D9=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="41" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="1" stopIfTrue="1">
       <formula>$B9=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="2">
+    <cfRule type="expression" dxfId="91" priority="2">
       <formula>$D9=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="4">
+    <cfRule type="expression" dxfId="90" priority="4">
       <formula>AND(B9&lt;&gt;1,D9=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="5">
+    <cfRule type="expression" dxfId="89" priority="5">
       <formula>AND($B9&lt;&gt;1,$D9&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3103,22 +3826,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D555DB45-06D3-4E53-8C52-4C0A4D00F5D5}">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="36"/>
-    <col min="2" max="2" width="26.5703125" style="36" customWidth="1"/>
-    <col min="3" max="3" width="56.35546875" style="36" customWidth="1"/>
-    <col min="4" max="4" width="25.0703125" style="36" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="36"/>
+    <col min="1" max="1" width="9.1796875" style="36"/>
+    <col min="2" max="2" width="26.54296875" style="36" customWidth="1"/>
+    <col min="3" max="3" width="56.36328125" style="36" customWidth="1"/>
+    <col min="4" max="4" width="25.08984375" style="36" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
         <v>21</v>
       </c>
@@ -3129,7 +3852,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="140.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="138" x14ac:dyDescent="0.25">
       <c r="A2" s="36">
         <v>1</v>
       </c>
@@ -3140,7 +3863,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="36">
         <v>2</v>
       </c>
@@ -3148,7 +3871,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="36">
         <v>4</v>
       </c>
@@ -3156,7 +3879,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="56" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A11" s="36">
         <v>5</v>
       </c>
@@ -3164,7 +3887,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="36">
         <v>6</v>
       </c>
@@ -3172,128 +3895,239 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="28" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A19" s="36">
         <v>7</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" s="36" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="126" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="124.2" x14ac:dyDescent="0.25">
       <c r="A22" s="36">
         <v>8</v>
       </c>
       <c r="B22" s="36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" s="36" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A25" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="36" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A28" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="36" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A30" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="36" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A34" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="36" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" s="36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="C38" s="40" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="55.2" x14ac:dyDescent="0.25">
+      <c r="A39" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="C39" s="36" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A42" s="36" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="B25" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" s="36" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="28" x14ac:dyDescent="0.3">
-      <c r="A28" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="B28" s="36" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="42" x14ac:dyDescent="0.3">
-      <c r="A30" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" s="36" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="28" x14ac:dyDescent="0.3">
-      <c r="A34" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="B34" s="36" t="s">
-        <v>58</v>
-      </c>
-      <c r="C34" s="36" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="C37" s="36" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="28" x14ac:dyDescent="0.3">
-      <c r="C38" s="40" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="56" x14ac:dyDescent="0.3">
-      <c r="A39" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="B39" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="C39" s="36" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="28" x14ac:dyDescent="0.3">
-      <c r="A42" s="36" t="s">
-        <v>67</v>
-      </c>
       <c r="B42" s="36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="36" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="36" t="s">
+      <c r="B45" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="B45" s="36" t="s">
+    </row>
+    <row r="47" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A47" s="36" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="28" x14ac:dyDescent="0.3">
-      <c r="A47" s="36" t="s">
+      <c r="B47" s="36" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="B47" s="36" t="s">
+      <c r="B49" s="36" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="36" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="B49" s="36" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="36" t="s">
-        <v>79</v>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C67"/>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C69"/>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="71" spans="3:3" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B88" s="50" t="s">
+        <v>97</v>
+      </c>
+      <c r="C88" s="48" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B89" s="51"/>
+      <c r="C89" s="48" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B90" s="51"/>
+      <c r="C90" s="48" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B91" s="51"/>
+      <c r="C91"/>
+    </row>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B92" s="51"/>
+      <c r="C92" s="48" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B93" s="51"/>
+      <c r="C93" s="48" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B94" s="52"/>
+      <c r="C94" s="49" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B88:B94"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="C38" r:id="rId1" xr:uid="{5C5B9DE7-052C-4C5F-828C-C463458523F2}"/>
   </hyperlinks>
@@ -3303,240 +4137,34 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C58DE228-9694-49AA-B7F0-62FF3C86A015}">
-  <dimension ref="A1:A19"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="82.78515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>92</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr codeName="TaskSetup">
-    <tabColor theme="6" tint="0.39997558519241921"/>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:O9"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="3.78515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="21" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" style="2" customWidth="1"/>
-    <col min="4" max="6" width="8.78515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="7.2109375" style="2" hidden="1" customWidth="1"/>
-    <col min="8" max="15" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="10.7109375" style="2" hidden="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:11" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="46" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="47" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="47"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-    </row>
-    <row r="2" spans="2:11" ht="83.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-    </row>
-    <row r="3" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-    </row>
-    <row r="4" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="5"/>
-    </row>
-    <row r="7" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="5"/>
-    </row>
-    <row r="8" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="5"/>
-      <c r="E8" s="25"/>
-    </row>
-    <row r="9" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="5"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:F1"/>
-  </mergeCells>
-  <phoneticPr fontId="27" type="noConversion"/>
-  <dataValidations count="4">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create an Assignment Setup in this worksheet. Insert or modify entries in Color Keys table starting in cell B4. Select cell G1 to navigate to To Do List. Tip is in cell B2" sqref="A1" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insert or modify Assigned To names in this column under this heading" sqref="B3" xr:uid="{00000000-0002-0000-0100-000002000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell, tip in cell below, and navigation link to To Do List worksheet in cell at right" sqref="B1" xr:uid="{00000000-0002-0000-0100-000003000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Navigation link to To Do List worksheet" sqref="E1 G1:K2" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
-  </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="G1:K2" location="'To Do List'!A1" tooltip="Select to navigate to To Do List worksheet" display="&lt; To Do List" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="E1:F1" location="'To Do List'!A1" tooltip="Click to navigate to To Do List worksheet" display="&lt; To Do List" xr:uid="{030E72E2-83DE-4827-9931-20D8B9FA68D2}"/>
-  </hyperlinks>
-  <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="65" fitToHeight="0" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69EEA948-B125-4EA3-895B-CADE82C01CA9}">
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q15"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.78515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="20.28515625" style="2" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" style="4" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="1.81640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="27.26953125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.7265625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="16.7265625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="18.54296875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="7.7265625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="20.26953125" style="2" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="17.26953125" style="4" hidden="1" customWidth="1"/>
     <col min="10" max="14" width="0" style="4" hidden="1" customWidth="1"/>
     <col min="15" max="17" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.7109375" style="2" hidden="1"/>
+    <col min="18" max="16384" width="10.7265625" style="2" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="66" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:17" ht="66" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -3559,11 +4187,11 @@
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
     </row>
-    <row r="2" spans="1:17" ht="21.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:17" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="12"/>
       <c r="B2" s="43">
         <f ca="1">TODAY()</f>
-        <v>44505</v>
+        <v>44598</v>
       </c>
       <c r="C2" s="43"/>
       <c r="D2" s="18"/>
@@ -3578,7 +4206,7 @@
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
     </row>
-    <row r="3" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="22" t="s">
         <v>9</v>
@@ -3599,7 +4227,7 @@
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
     </row>
-    <row r="4" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="22" t="s">
         <v>10</v>
@@ -3621,7 +4249,7 @@
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
     </row>
-    <row r="5" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="7"/>
       <c r="C5" s="14"/>
       <c r="D5" s="11"/>
@@ -3635,7 +4263,7 @@
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
     </row>
-    <row r="6" spans="1:17" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15"/>
       <c r="B6" s="24" t="s">
         <v>2</v>
@@ -3659,7 +4287,7 @@
       <c r="N6" s="15"/>
       <c r="O6" s="15"/>
     </row>
-    <row r="7" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="42" t="s">
         <v>12</v>
       </c>
@@ -3667,7 +4295,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="1"/>
@@ -3679,13 +4307,13 @@
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="42"/>
       <c r="B8" s="9">
         <v>0</v>
       </c>
       <c r="C8" s="41" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="1"/>
@@ -3697,7 +4325,7 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="42"/>
       <c r="B9" s="9">
         <v>0</v>
@@ -3715,12 +4343,12 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="9">
         <v>0</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="1"/>
@@ -3732,7 +4360,7 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="9"/>
       <c r="C11" s="8" t="s">
         <v>35</v>
@@ -3747,10 +4375,10 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="9"/>
       <c r="C12" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D12" s="30"/>
       <c r="E12" s="1"/>
@@ -3762,10 +4390,10 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="9"/>
       <c r="C13" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="1"/>
@@ -3777,7 +4405,7 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -3785,7 +4413,10 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>104</v>
+      </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -3793,98 +4424,118 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
     </row>
+    <row r="16" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="A7:A9"/>
   </mergeCells>
   <conditionalFormatting sqref="C11:C12 C9">
-    <cfRule type="expression" dxfId="29" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="33" stopIfTrue="1">
       <formula>D9=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:F12 D13:F13 D7:F9 C9">
-    <cfRule type="expression" dxfId="28" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="31" stopIfTrue="1">
       <formula>$B7=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="32">
+    <cfRule type="expression" dxfId="80" priority="32">
       <formula>$D7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="34">
+    <cfRule type="expression" dxfId="79" priority="34">
       <formula>AND(B7&lt;&gt;1,D7=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="35">
+    <cfRule type="expression" dxfId="78" priority="35">
       <formula>AND($B7&lt;&gt;1,$D7&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="expression" dxfId="24" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="28" stopIfTrue="1">
       <formula>D7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="expression" dxfId="23" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="26" stopIfTrue="1">
       <formula>$B7=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="27">
+    <cfRule type="expression" dxfId="75" priority="27">
       <formula>$D7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="29">
+    <cfRule type="expression" dxfId="74" priority="29">
       <formula>AND(B7&lt;&gt;1,D7=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="30">
+    <cfRule type="expression" dxfId="73" priority="30">
       <formula>AND($B7&lt;&gt;1,$D7&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="expression" dxfId="19" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="13" stopIfTrue="1">
       <formula>D8=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="expression" dxfId="18" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="11" stopIfTrue="1">
       <formula>$B8=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="12">
+    <cfRule type="expression" dxfId="70" priority="12">
       <formula>$D8=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="14">
+    <cfRule type="expression" dxfId="69" priority="14">
       <formula>AND(B8&lt;&gt;1,D8=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="15">
+    <cfRule type="expression" dxfId="68" priority="15">
       <formula>AND($B8&lt;&gt;1,$D8&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:F10">
-    <cfRule type="expression" dxfId="14" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="6" stopIfTrue="1">
       <formula>$B10=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="7">
+    <cfRule type="expression" dxfId="66" priority="7">
       <formula>$D10=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="8">
+    <cfRule type="expression" dxfId="65" priority="8">
       <formula>AND(C10&lt;&gt;1,E10=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="9">
+    <cfRule type="expression" dxfId="64" priority="9">
       <formula>AND($B10&lt;&gt;1,$D10&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="10" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="3" stopIfTrue="1">
       <formula>D10=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="9" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="1" stopIfTrue="1">
       <formula>$B10=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="2">
+    <cfRule type="expression" dxfId="61" priority="2">
       <formula>$D10=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="60" priority="4">
       <formula>AND(B10&lt;&gt;1,D10=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="59" priority="5">
       <formula>AND($B10&lt;&gt;1,$D10&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3967,7 +4618,873 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2B0A940-E58C-4F73-B098-D84B75D771FF}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.59999389629810485"/>
+    <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:Q17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="1.81640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="27.26953125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.7265625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="16.7265625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="18.54296875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="7.7265625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="20.26953125" style="2" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="17.26953125" style="4" hidden="1" customWidth="1"/>
+    <col min="10" max="14" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="15" max="17" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.7265625" style="2" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="66" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="19"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+    </row>
+    <row r="2" spans="1:17" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="12"/>
+      <c r="B2" s="43">
+        <f ca="1">TODAY()</f>
+        <v>44598</v>
+      </c>
+      <c r="C2" s="43"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+    </row>
+    <row r="3" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="23">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+    </row>
+    <row r="4" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="23">
+        <f ca="1">COUNTIFS(ToDoList4[Due Date],"&lt;"&amp;TODAY(),ToDoList4[Done],"&lt;&gt;1")</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+    </row>
+    <row r="5" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="7"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:17" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+      <c r="B6" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+    </row>
+    <row r="7" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="9">
+        <v>1</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="6">
+        <f ca="1">TODAY()-1</f>
+        <v>44597</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="42"/>
+      <c r="B8" s="9">
+        <v>1</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="6">
+        <f ca="1">TODAY()+2</f>
+        <v>44600</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="42"/>
+      <c r="B9" s="9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="6">
+        <f ca="1">TODAY()+1</f>
+        <v>44599</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="42"/>
+      <c r="B10" s="9">
+        <v>1</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="6">
+        <f ca="1">TODAY()+1</f>
+        <v>44599</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="42"/>
+      <c r="B11" s="9">
+        <v>1</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="6">
+        <f ca="1">TODAY()+2</f>
+        <v>44600</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="9">
+        <v>1</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="6">
+        <f ca="1">TODAY()+8</f>
+        <v>44606</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="32">
+        <v>1</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="34">
+        <f ca="1">TODAY()+5</f>
+        <v>44603</v>
+      </c>
+      <c r="E13" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="9"/>
+      <c r="C14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="6">
+        <f ca="1">TODAY()+2</f>
+        <v>44600</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="9"/>
+      <c r="C15" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="6">
+        <f ca="1">TODAY()+2</f>
+        <v>44600</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="9">
+        <v>1</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="6">
+        <f ca="1">TODAY()+3</f>
+        <v>44601</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="2:6" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="32">
+        <v>1</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="6">
+        <f ca="1">TODAY()+3</f>
+        <v>44601</v>
+      </c>
+      <c r="E17" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="39" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="A7:A11"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C7:C8 C14:C15 C11:C12">
+    <cfRule type="expression" dxfId="52" priority="48" stopIfTrue="1">
+      <formula>D7=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7:F8 C14:F15 C11:F12">
+    <cfRule type="expression" dxfId="51" priority="46" stopIfTrue="1">
+      <formula>$B7=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="50" priority="47">
+      <formula>$D7=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="49" priority="49">
+      <formula>AND(B7&lt;&gt;1,D7=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="48" priority="50">
+      <formula>AND($B7&lt;&gt;1,$D7&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16">
+    <cfRule type="expression" dxfId="47" priority="34" stopIfTrue="1">
+      <formula>D16=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F16">
+    <cfRule type="expression" dxfId="46" priority="41" stopIfTrue="1">
+      <formula>$B16=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="45" priority="42">
+      <formula>$D16=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="43">
+      <formula>AND(E16&lt;&gt;1,G16=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="43" priority="44">
+      <formula>AND($B16&lt;&gt;1,$D16&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16">
+    <cfRule type="expression" dxfId="42" priority="37" stopIfTrue="1">
+      <formula>$B16=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="41" priority="38">
+      <formula>$D16=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="39">
+      <formula>AND(C16&lt;&gt;1,E16=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="39" priority="40">
+      <formula>AND($B16&lt;&gt;1,$D16&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16">
+    <cfRule type="expression" dxfId="38" priority="32" stopIfTrue="1">
+      <formula>$B16=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="33">
+      <formula>$D16=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="35">
+      <formula>AND(B16&lt;&gt;1,D16=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="35" priority="36">
+      <formula>AND($B16&lt;&gt;1,$D16&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16">
+    <cfRule type="expression" dxfId="34" priority="28" stopIfTrue="1">
+      <formula>$B16=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="29">
+      <formula>$D16=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="30">
+      <formula>AND(D16&lt;&gt;1,F16=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="31" priority="31">
+      <formula>AND($B16&lt;&gt;1,$D16&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="expression" dxfId="30" priority="24" stopIfTrue="1">
+      <formula>D13=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13:F13">
+    <cfRule type="expression" dxfId="29" priority="22" stopIfTrue="1">
+      <formula>$B13=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="23">
+      <formula>$D13=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="25">
+      <formula>AND(B13&lt;&gt;1,D13=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="26">
+      <formula>AND($B13&lt;&gt;1,$D13&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9:F9">
+    <cfRule type="expression" dxfId="25" priority="17" stopIfTrue="1">
+      <formula>$B9=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="18">
+      <formula>$D9=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="23" priority="19">
+      <formula>AND(C9&lt;&gt;1,E9=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="20">
+      <formula>AND($B9&lt;&gt;1,$D9&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10">
+    <cfRule type="expression" dxfId="21" priority="13" stopIfTrue="1">
+      <formula>D10=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10:F10">
+    <cfRule type="expression" dxfId="20" priority="11" stopIfTrue="1">
+      <formula>$B10=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="12">
+      <formula>$D10=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="14">
+      <formula>AND(B10&lt;&gt;1,D10=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="15">
+      <formula>AND($B10&lt;&gt;1,$D10&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="expression" dxfId="16" priority="8" stopIfTrue="1">
+      <formula>D9=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="expression" dxfId="15" priority="6" stopIfTrue="1">
+      <formula>$B9=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="7">
+      <formula>$D9=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="9">
+      <formula>AND(B9&lt;&gt;1,D9=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="10">
+      <formula>AND($B9&lt;&gt;1,$D9&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17">
+    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
+      <formula>$B17=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>$D17=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>AND(C17&lt;&gt;1,E17=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="4">
+      <formula>AND($B17&lt;&gt;1,$D17&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="17">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select Assigned to names from the list. Select CANCEL, press ALT+DOWN ARROW for options, then DOWN ARROW and ENTER to make selection" sqref="F7:F17" xr:uid="{2FE444E8-B9F6-4A2B-BF95-B4C274A4F32D}">
+      <formula1>Assignedto</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select Priority from the list. Select CANCEL, press ALT+DOWN ARROW for options, then DOWN ARROW and ENTER to make selection" sqref="E7:E17" xr:uid="{3B7DA989-D9D7-45EB-A694-4BBC2A902FFB}">
+      <formula1>"High,Medium,Low"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="B5:C5" xr:uid="{C80793E2-BB46-4DF4-BC7C-50CAD9A525FB}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Overdue days are automatically updated in this cell. Enter details in table below. Table tip is in cell A6" sqref="C4" xr:uid="{8C640474-7820-4D3F-9B99-3124A4B62D1B}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Overdue days are automatically updated in cell at right" sqref="B4" xr:uid="{9FF29D43-B882-48D7-A5C6-895A87573A2F}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this C1. Date is automatically updated in cell B2, and Due Today and Overdue days in cell C3 and C4. Next tip is in cell below." sqref="B1" xr:uid="{C9E2F777-7448-4815-BC40-CF6E5F5D31C9}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell. Date is automatically updated in cell below, and Due Today and Overdue days in cell C3 and C4. Tip is in cell at right" sqref="C1" xr:uid="{0AFD76E5-F21C-4082-8C06-220E2A6042B6}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter value greater than 1 in this column under this heading to mark task as Done. Strikethrough formatting will automatically be applied" sqref="B6" xr:uid="{7EBE5C21-1ABC-48B2-910B-E213B3B96339}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select Assigned to names in this column under this heading. Press ALT+DOWN ARROW for options, then DOWN ARROW and ENTER to make selection" sqref="F6" xr:uid="{8A986117-9AC1-4C35-913B-286C57793C6C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select Priority in this column under this heading. Press ALT+DOWN ARROW for options, then DOWN ARROW and ENTER to make selection" sqref="E6" xr:uid="{11578A6A-BC58-4B58-927F-B2AD77DF2DFB}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Due Date in this column under this heading" sqref="D6" xr:uid="{08A06C66-56C5-48EA-8EB5-7241BF42BB9F}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Description in this column under this heading" sqref="C6" xr:uid="{8F8AA43C-4537-4612-8670-B809F8344078}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Due Today is automatically updated in this cell" sqref="C3" xr:uid="{67DB34A8-F864-473A-9365-C2BA853A7DB1}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Due Today is automatically updated in cell at right" sqref="B3" xr:uid="{64737FC3-EA72-4D82-9EB8-D15605E525AB}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Date is automatically updated in this cell and Due Today and Overdue days in cells below" sqref="B2:C2" xr:uid="{84A5C09C-FDE8-4D09-825F-238FFD61029F}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Navigation link to Assignment Setup worksheet" sqref="F1:G5" xr:uid="{F14332AA-C40D-42B2-8F6A-5CB94690F507}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create To Do List in this workbook. Enter details in To Do List table in this worksheet. Select cell F1 to navigate to Setup worksheet. Due &amp; Overdue days are automatically updated" sqref="A1" xr:uid="{660D059F-77C3-4234-920E-178B4B39853B}"/>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="F1" location="'Assignment Setup'!A1" tooltip="Click to navigate to TAssignment Setup" display="Setup &gt;" xr:uid="{4B637F1B-0B81-4292-B3A4-1E773EF0C176}"/>
+  </hyperlinks>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="58" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="51" id="{B865E691-8D2C-44A3-8FD3-18BE1230F257}">
+            <x14:iconSet iconSet="3Symbols2" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="formula">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>B7:B8 B14:B15 B11:B12</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="45" id="{1E829A64-0D67-48C9-AB6D-B403E2893716}">
+            <x14:iconSet iconSet="3Symbols2" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="formula">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>B16</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="27" id="{0D627A13-EEB7-4F63-AE4C-E8D1944F28AB}">
+            <x14:iconSet iconSet="3Symbols2" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="formula">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>B13</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="21" id="{964B918D-4811-482A-B0CF-38BB73069508}">
+            <x14:iconSet iconSet="3Symbols2" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="formula">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>B9</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="16" id="{933904E7-1814-4C90-9E7C-81BC06108A3B}">
+            <x14:iconSet iconSet="3Symbols2" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="formula">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>B10</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="5" id="{0F83DF3A-A6A3-4778-8500-28481AEDC69C}">
+            <x14:iconSet iconSet="3Symbols2" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="formula">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>B17</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="TaskSetup">
+    <tabColor theme="6" tint="0.39997558519241921"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:O9"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.81640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="21" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.26953125" style="2" customWidth="1"/>
+    <col min="4" max="6" width="8.81640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="7.1796875" style="2" hidden="1" customWidth="1"/>
+    <col min="8" max="15" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="16" max="16384" width="10.7265625" style="2" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="47"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+    </row>
+    <row r="2" spans="2:11" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+    </row>
+    <row r="3" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+    </row>
+    <row r="4" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="5"/>
+    </row>
+    <row r="7" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+    </row>
+    <row r="8" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="5"/>
+      <c r="E8" s="25"/>
+    </row>
+    <row r="9" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
+  <phoneticPr fontId="27" type="noConversion"/>
+  <dataValidations count="4">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create an Assignment Setup in this worksheet. Insert or modify entries in Color Keys table starting in cell B4. Select cell G1 to navigate to To Do List. Tip is in cell B2" sqref="A1" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insert or modify Assigned To names in this column under this heading" sqref="B3" xr:uid="{00000000-0002-0000-0100-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell, tip in cell below, and navigation link to To Do List worksheet in cell at right" sqref="B1" xr:uid="{00000000-0002-0000-0100-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Navigation link to To Do List worksheet" sqref="E1 G1:K2" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="G1:K2" location="'To Do List'!A1" tooltip="Select to navigate to To Do List worksheet" display="&lt; To Do List" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="E1:F1" location="'To Do List'!A1" tooltip="Click to navigate to To Do List worksheet" display="&lt; To Do List" xr:uid="{030E72E2-83DE-4827-9931-20D8B9FA68D2}"/>
+  </hyperlinks>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="65" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -3976,7 +5493,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DEEA25CC0A0AC24199CDC46C25B8B0BC" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e3b47856d4cf355c0dacb39e1084d14f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="6dc4bcd6-49db-4c07-9060-8acfc67cef9f" xmlns:ns3="fb0879af-3eba-417a-a55a-ffe6dcd6ca77" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a845a615265fdb1f7b12cc65ac20ecbd" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4184,16 +5701,17 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03CCC4C8-6A95-4999-B963-115A022CA31F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{920DC3BD-3C4B-4C78-91FF-63EB10F70D2C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -4201,7 +5719,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7118F064-9046-4DCB-A010-2D274D0FB549}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4219,14 +5737,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03CCC4C8-6A95-4999-B963-115A022CA31F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Monday motivation || Restructured QuizApp excel sheet
</commit_message>
<xml_diff>
--- a/App_Data/QuizApplication.xlsx
+++ b/App_Data/QuizApplication.xlsx
@@ -3,19 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD7B907-F813-44F3-898A-5488D10BF0B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA9346E-71F7-40C9-86CE-57E8B9A8D022}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1210" yWindow="-110" windowWidth="18100" windowHeight="11020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="-108" windowWidth="22128" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="To Do List - POC" sheetId="7" r:id="rId1"/>
-    <sheet name="Questions" sheetId="8" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="10" r:id="rId3"/>
-    <sheet name="Assignment Setup" sheetId="6" r:id="rId4"/>
-    <sheet name="To Do List-RoadMap" sheetId="9" r:id="rId5"/>
+    <sheet name="To Do List" sheetId="7" r:id="rId1"/>
+    <sheet name="To Do - Details" sheetId="8" r:id="rId2"/>
+    <sheet name="FunApp-RoadMap" sheetId="9" r:id="rId3"/>
+    <sheet name="2021_WorkProgress" sheetId="11" r:id="rId4"/>
+    <sheet name="Assignment Setup" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="Assignedto" localSheetId="4">ColorKeys[Assigned To]</definedName>
+    <definedName name="Assignedto" localSheetId="3">ColorKeys[Assigned To]</definedName>
+    <definedName name="Assignedto" localSheetId="2">ColorKeys[Assigned To]</definedName>
     <definedName name="Assignedto">ColorKeys[Assigned To]</definedName>
     <definedName name="Color1">'Assignment Setup'!$B$4</definedName>
     <definedName name="Color2">'Assignment Setup'!$B$5</definedName>
@@ -23,18 +24,24 @@
     <definedName name="Color4">'Assignment Setup'!$B$7</definedName>
     <definedName name="Color5">'Assignment Setup'!$B$8</definedName>
     <definedName name="Color6">'Assignment Setup'!$B$9</definedName>
-    <definedName name="ColorKey" localSheetId="4">ColorKeys[Assigned To]</definedName>
+    <definedName name="ColorKey" localSheetId="3">ColorKeys[Assigned To]</definedName>
+    <definedName name="ColorKey" localSheetId="2">ColorKeys[Assigned To]</definedName>
     <definedName name="ColorKey">ColorKeys[Assigned To]</definedName>
-    <definedName name="ColumnTitle1" localSheetId="4">ToDoList2[[#Headers],[Done]]</definedName>
+    <definedName name="ColumnTitle1" localSheetId="3">ToDoList4[[#Headers],[Done]]</definedName>
+    <definedName name="ColumnTitle1" localSheetId="2">ToDoList2[[#Headers],[Done]]</definedName>
     <definedName name="ColumnTitle1">ToDoList[[#Headers],[Done]]</definedName>
-    <definedName name="ColumnTitle2" localSheetId="4">ColorKeys[[#Headers],[Assigned To]]</definedName>
+    <definedName name="ColumnTitle2" localSheetId="3">ColorKeys[[#Headers],[Assigned To]]</definedName>
+    <definedName name="ColumnTitle2" localSheetId="2">ColorKeys[[#Headers],[Assigned To]]</definedName>
     <definedName name="ColumnTitle2">ColorKeys[[#Headers],[Assigned To]]</definedName>
-    <definedName name="DueToday" localSheetId="4">'To Do List-RoadMap'!$C$3</definedName>
-    <definedName name="DueToday">'To Do List - POC'!$C$3</definedName>
+    <definedName name="DueToday" localSheetId="3">'2021_WorkProgress'!$C$3</definedName>
+    <definedName name="DueToday" localSheetId="2">'FunApp-RoadMap'!$C$3</definedName>
+    <definedName name="DueToday">'To Do List'!$C$3</definedName>
+    <definedName name="Grid" localSheetId="3">ToDoList4[[#All],[Description]:[Assigned to]]</definedName>
+    <definedName name="Grid" localSheetId="2">ToDoList2[[#All],[Description]:[Assigned to]]</definedName>
     <definedName name="Grid" localSheetId="0">ToDoList[[#All],[Description]:[Assigned to]]</definedName>
-    <definedName name="Grid" localSheetId="4">ToDoList2[[#All],[Description]:[Assigned to]]</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'To Do List - POC'!$1:$6</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="4">'To Do List-RoadMap'!$1:$6</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="3">'2021_WorkProgress'!$1:$6</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="2">'FunApp-RoadMap'!$1:$6</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'To Do List'!$1:$6</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -52,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="109">
   <si>
     <t xml:space="preserve">                            </t>
   </si>
@@ -200,9 +207,6 @@
     <t>Panda</t>
   </si>
   <si>
-    <t xml:space="preserve">Technical Expert </t>
-  </si>
-  <si>
     <t xml:space="preserve">Developer </t>
   </si>
   <si>
@@ -358,9 +362,6 @@
     <t>7.Hint Section on the top: Disappear the two answer list</t>
   </si>
   <si>
-    <t>--------------------</t>
-  </si>
-  <si>
     <t>https://github.com/mattboldt/typed.js/issues/396</t>
   </si>
   <si>
@@ -368,6 +369,57 @@
   </si>
   <si>
     <t>ToDo</t>
+  </si>
+  <si>
+    <t>Display who answered first on submit</t>
+  </si>
+  <si>
+    <t>Server response using Signal R</t>
+  </si>
+  <si>
+    <t>Rajish and Asish</t>
+  </si>
+  <si>
+    <t>Admin Page Display (CRUD)</t>
+  </si>
+  <si>
+    <t>Defect Fix (Please look into To-Do Details)</t>
+  </si>
+  <si>
+    <t>From Raghu?</t>
+  </si>
+  <si>
+    <t>Infrastructure</t>
+  </si>
+  <si>
+    <t>1. Web Server where we can host website</t>
+  </si>
+  <si>
+    <t>2. SQL DataBase to Deploy the DB</t>
+  </si>
+  <si>
+    <t>Future:</t>
+  </si>
+  <si>
+    <t>Enable the url without VPN with token</t>
+  </si>
+  <si>
+    <t>Android App using DotNet</t>
+  </si>
+  <si>
+    <t>Steps to add Questions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. Add the QuestionGroup Name in Quiz table</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2. Add a question in Questions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3. Add the AnswerChoices in  the [Choices] table with the corresponding question identity value</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4. Add a record for Answers in the Answers Table</t>
   </si>
 </sst>
 </file>
@@ -381,7 +433,7 @@
     <numFmt numFmtId="167" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
     <numFmt numFmtId="168" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.14996795556505021"/>
@@ -602,6 +654,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF262626"/>
+      <name val="Lucida Sans"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -635,7 +694,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -672,6 +731,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFC8F0FF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="6" tint="0.79998168889431442"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1">
@@ -691,7 +768,7 @@
     <xf numFmtId="167" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="14" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -828,6 +905,21 @@
     <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="20% - Accent5" xfId="1" builtinId="46"/>
@@ -843,7 +935,58 @@
     <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="8" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="85">
+  <dxfs count="136">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <u val="none"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="6" tint="0.79998168889431442"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <name val="Rockwell"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -942,6 +1085,11 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <color auto="1"/>
       </font>
     </dxf>
@@ -972,11 +1120,6 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="3"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <color auto="1"/>
       </font>
     </dxf>
@@ -1042,15 +1185,150 @@
     </dxf>
     <dxf>
       <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <u val="none"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <u val="none"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <u val="none"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="3"/>
       </font>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="6" tint="0.79998168889431442"/>
-        </bottom>
-      </border>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <u val="none"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="&quot;Done&quot;;&quot;&quot;;&quot;&quot;"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1059,11 +1337,181 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="0"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.14996795556505021"/>
         <name val="Rockwell"/>
         <family val="1"/>
         <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <u val="none"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <u val="none"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <u val="none"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <u val="none"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <u val="none"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
       </font>
     </dxf>
     <dxf>
@@ -1478,14 +1926,14 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="To Do List" defaultPivotStyle="PivotStyleLight18">
     <tableStyle name="Address Book" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="84"/>
-      <tableStyleElement type="headerRow" dxfId="83"/>
-      <tableStyleElement type="firstRowStripe" dxfId="82"/>
-      <tableStyleElement type="secondRowStripe" dxfId="81"/>
+      <tableStyleElement type="wholeTable" dxfId="135"/>
+      <tableStyleElement type="headerRow" dxfId="134"/>
+      <tableStyleElement type="firstRowStripe" dxfId="133"/>
+      <tableStyleElement type="secondRowStripe" dxfId="132"/>
     </tableStyle>
     <tableStyle name="To Do List" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="80"/>
-      <tableStyleElement type="headerRow" dxfId="79"/>
+      <tableStyleElement type="wholeTable" dxfId="131"/>
+      <tableStyleElement type="headerRow" dxfId="130"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -2130,15 +2578,327 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>990600</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>21600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Data Entry Tip" descr="Enter a number greater than 1 in Done column when  task is complete">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5020EA12-0F30-4F68-8E17-BAB8C6D2EE1F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3406140" y="1112520"/>
+          <a:ext cx="990600" cy="600720"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="72000" tIns="0" rIns="72000" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="800">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Enter a number 1 in Done column when  task is complete</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData fPrintsWithSheet="0"/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>21600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Data Entry Tip" descr="Enter a number greater than 1 in Done column when  task is complete">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B016A975-C429-4676-9694-847F614094F9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4434840" y="1112520"/>
+          <a:ext cx="2194560" cy="600720"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="72000" tIns="0" rIns="72000" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="800">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Select</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="800" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> a drop down arrow, such as </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="800">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Assigned To or Priority,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="800" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="800">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>to Filter or Sort your To Do List items.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="800">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="800">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>T</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="800" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>ips </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="800">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>do not print.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="800">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData fPrintsWithSheet="0"/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>177512</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>111667</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>626669</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>762687</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="Decorative element&#10;">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D70D7AAB-B1E3-4AF3-B349-26858E2CF24B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm rot="21012350">
+          <a:off x="329912" y="111667"/>
+          <a:ext cx="449157" cy="651020"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ToDoList" displayName="ToDoList" ref="B6:F17" totalsRowShown="0" headerRowDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ToDoList" displayName="ToDoList" ref="B6:F17" totalsRowShown="0" headerRowDxfId="88">
   <autoFilter ref="B6:F17" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Done" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Description" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Due Date" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Priority" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Assigned to" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Done" dataDxfId="87"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Description" dataDxfId="86"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Due Date" dataDxfId="85"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Priority" dataDxfId="84"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Assigned to" dataDxfId="83"/>
   </tableColumns>
   <tableStyleInfo name="Address Book" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2150,7 +2910,45 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="ColorKeys" displayName="ColorKeys" ref="B3:C9" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EAB70A46-0CF0-4D35-9438-FC09BD356BF6}" name="ToDoList2" displayName="ToDoList2" ref="B6:F13" totalsRowShown="0" headerRowDxfId="58">
+  <autoFilter ref="B6:F13" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{6D55EE3E-E775-41B3-BC0A-08AC46F6EF17}" name="Done" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{A568071C-C7BC-49A3-A2AE-BC0A89D3D4A4}" name="Description" dataDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{BE941CF0-BB93-4A44-A031-79654E12770C}" name="Due Date" dataDxfId="55"/>
+    <tableColumn id="4" xr3:uid="{198586D7-EC80-4B60-A7EF-306798680CD2}" name="Priority" dataDxfId="54"/>
+    <tableColumn id="5" xr3:uid="{ECB977EA-E1B7-4EE3-9E79-1070BBA35C42}" name="Assigned to" dataDxfId="53"/>
+  </tableColumns>
+  <tableStyleInfo name="Address Book" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{504A1905-F514-4f6f-8877-14C23A59335A}">
+      <x14:table altTextSummary="Enter 1 to mark task as Done, Description, and Due Date, and select Priority and Assigned to names in this table"/>
+    </ext>
+  </extLst>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AE7EE83F-8E62-4BCF-B169-EBD3D0E85BEF}" name="ToDoList4" displayName="ToDoList4" ref="B6:F17" totalsRowShown="0" headerRowDxfId="11">
+  <autoFilter ref="B6:F17" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{6822DCC8-0392-486B-8480-4FB115516904}" name="Done" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{4942A3B4-C013-4609-95C7-B7BF88BDEE37}" name="Description" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{0C52536F-1EFF-49FC-8E87-5789F5F15AD5}" name="Due Date" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{7D2DCE90-A34A-4881-B20D-2D149D62374F}" name="Priority" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{D881DC46-F30D-426B-8535-304AF38351F1}" name="Assigned to" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="Address Book" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{504A1905-F514-4f6f-8877-14C23A59335A}">
+      <x14:table altTextSummary="Enter 1 to mark task as Done, Description, and Due Date, and select Priority and Assigned to names in this table"/>
+    </ext>
+  </extLst>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="ColorKeys" displayName="ColorKeys" ref="B3:C9" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4">
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Assigned To"/>
     <tableColumn id="2" xr3:uid="{F36E0378-7DB9-42F4-B4F4-263BE6500357}" name="Column1"/>
@@ -2159,25 +2957,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{504A1905-F514-4f6f-8877-14C23A59335A}">
       <x14:table altTextSummary="Insert or modify Assigned To names in this table"/>
-    </ext>
-  </extLst>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EAB70A46-0CF0-4D35-9438-FC09BD356BF6}" name="ToDoList2" displayName="ToDoList2" ref="B6:F13" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="B6:F13" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{6D55EE3E-E775-41B3-BC0A-08AC46F6EF17}" name="Done" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{A568071C-C7BC-49A3-A2AE-BC0A89D3D4A4}" name="Description" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{BE941CF0-BB93-4A44-A031-79654E12770C}" name="Due Date" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{198586D7-EC80-4B60-A7EF-306798680CD2}" name="Priority" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{ECB977EA-E1B7-4EE3-9E79-1070BBA35C42}" name="Assigned to" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="Address Book" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{504A1905-F514-4f6f-8877-14C23A59335A}">
-      <x14:table altTextSummary="Enter 1 to mark task as Done, Description, and Due Date, and select Priority and Assigned to names in this table"/>
     </ext>
   </extLst>
 </table>
@@ -2416,27 +3195,27 @@
   </sheetPr>
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.78515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="20.28515625" style="2" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" style="4" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="1.81640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="27.26953125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.7265625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="16.7265625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="18.54296875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="7.7265625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="20.26953125" style="2" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="17.26953125" style="4" hidden="1" customWidth="1"/>
     <col min="10" max="14" width="0" style="4" hidden="1" customWidth="1"/>
     <col min="15" max="17" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.7109375" style="2" hidden="1"/>
+    <col min="18" max="16384" width="10.7265625" style="2" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="66" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:17" ht="66" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -2459,11 +3238,11 @@
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
     </row>
-    <row r="2" spans="1:17" ht="21.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:17" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="12"/>
       <c r="B2" s="43">
         <f ca="1">TODAY()</f>
-        <v>44505</v>
+        <v>44598</v>
       </c>
       <c r="C2" s="43"/>
       <c r="D2" s="18"/>
@@ -2478,7 +3257,7 @@
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
     </row>
-    <row r="3" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="22" t="s">
         <v>9</v>
@@ -2499,7 +3278,7 @@
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
     </row>
-    <row r="4" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="22" t="s">
         <v>10</v>
@@ -2521,7 +3300,7 @@
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
     </row>
-    <row r="5" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="7"/>
       <c r="C5" s="14"/>
       <c r="D5" s="11"/>
@@ -2535,7 +3314,7 @@
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
     </row>
-    <row r="6" spans="1:17" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15"/>
       <c r="B6" s="24" t="s">
         <v>2</v>
@@ -2559,19 +3338,19 @@
       <c r="N6" s="15"/>
       <c r="O6" s="15"/>
     </row>
-    <row r="7" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="42" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>18</v>
+        <v>92</v>
       </c>
       <c r="D7" s="6">
-        <f ca="1">TODAY()-1</f>
-        <v>44504</v>
+        <f ca="1">TODAY()+11</f>
+        <v>44609</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>5</v>
@@ -2586,23 +3365,23 @@
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="42"/>
       <c r="B8" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>20</v>
+        <v>93</v>
       </c>
       <c r="D8" s="6">
-        <f ca="1">TODAY()+2</f>
-        <v>44507</v>
+        <f ca="1">TODAY()+15</f>
+        <v>44613</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -2611,23 +3390,23 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="42"/>
       <c r="B9" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
       <c r="D9" s="6">
-        <f ca="1">TODAY()+1</f>
-        <v>44506</v>
+        <f ca="1">TODAY()+20</f>
+        <v>44618</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -2636,23 +3415,23 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="42"/>
       <c r="B10" s="9">
         <v>0</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>42</v>
+        <v>96</v>
       </c>
       <c r="D10" s="6">
-        <f ca="1">TODAY()+1</f>
-        <v>44506</v>
+        <f ca="1">TODAY()+20</f>
+        <v>44618</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>26</v>
+        <v>94</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -2661,24 +3440,15 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="42"/>
       <c r="B11" s="9">
-        <v>1</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="6">
-        <f ca="1">TODAY()+2</f>
-        <v>44507</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>26</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -2686,23 +3456,14 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="9">
-        <v>1</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="6">
-        <f ca="1">TODAY()+8</f>
-        <v>44513</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -2710,23 +3471,14 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="32">
-        <v>1</v>
-      </c>
-      <c r="C13" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="34">
-        <f ca="1">TODAY()+5</f>
-        <v>44510</v>
-      </c>
-      <c r="E13" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="35" t="s">
-        <v>38</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C13" s="33"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -2734,21 +3486,12 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="9"/>
-      <c r="C14" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="6">
-        <f ca="1">TODAY()+2</f>
-        <v>44507</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -2756,21 +3499,12 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="9"/>
-      <c r="C15" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="6">
-        <f ca="1">TODAY()+2</f>
-        <v>44507</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -2778,21 +3512,12 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
     </row>
-    <row r="16" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="9"/>
-      <c r="C16" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="6">
-        <f ca="1">TODAY()+3</f>
-        <v>44508</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -2800,11 +3525,9 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="2:6" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="37"/>
-      <c r="C17" s="31" t="s">
-        <v>56</v>
-      </c>
+      <c r="C17" s="31"/>
       <c r="D17" s="38"/>
       <c r="E17" s="39"/>
       <c r="F17" s="39"/>
@@ -2815,153 +3538,153 @@
     <mergeCell ref="B2:C2"/>
   </mergeCells>
   <conditionalFormatting sqref="C7:C8 C14:C15 C11:C12">
-    <cfRule type="expression" dxfId="78" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="129" priority="45" stopIfTrue="1">
       <formula>D7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:F8 C14:F15 C11:F12">
-    <cfRule type="expression" dxfId="77" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="128" priority="43" stopIfTrue="1">
       <formula>$B7=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="44">
+    <cfRule type="expression" dxfId="127" priority="44">
       <formula>$D7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="46">
+    <cfRule type="expression" dxfId="126" priority="46">
       <formula>AND(B7&lt;&gt;1,D7=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="47">
+    <cfRule type="expression" dxfId="125" priority="47">
       <formula>AND($B7&lt;&gt;1,$D7&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="73" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="124" priority="30" stopIfTrue="1">
       <formula>D16=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16">
-    <cfRule type="expression" dxfId="72" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="123" priority="37" stopIfTrue="1">
       <formula>$B16=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="38">
+    <cfRule type="expression" dxfId="122" priority="38">
       <formula>$D16=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="40">
+    <cfRule type="expression" dxfId="121" priority="40">
       <formula>AND(E16&lt;&gt;1,G16=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="41">
+    <cfRule type="expression" dxfId="120" priority="41">
       <formula>AND($B16&lt;&gt;1,$D16&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16">
-    <cfRule type="expression" dxfId="68" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="119" priority="33" stopIfTrue="1">
       <formula>$B16=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="34">
+    <cfRule type="expression" dxfId="118" priority="34">
       <formula>$D16=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="35">
+    <cfRule type="expression" dxfId="117" priority="35">
       <formula>AND(C16&lt;&gt;1,E16=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="36">
+    <cfRule type="expression" dxfId="116" priority="36">
       <formula>AND($B16&lt;&gt;1,$D16&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="64" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="115" priority="28" stopIfTrue="1">
       <formula>$B16=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="29">
+    <cfRule type="expression" dxfId="114" priority="29">
       <formula>$D16=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="31">
+    <cfRule type="expression" dxfId="113" priority="31">
       <formula>AND(B16&lt;&gt;1,D16=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="32">
+    <cfRule type="expression" dxfId="112" priority="32">
       <formula>AND($B16&lt;&gt;1,$D16&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="expression" dxfId="60" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="111" priority="24" stopIfTrue="1">
       <formula>$B16=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="25">
+    <cfRule type="expression" dxfId="110" priority="25">
       <formula>$D16=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="26">
+    <cfRule type="expression" dxfId="109" priority="26">
       <formula>AND(D16&lt;&gt;1,F16=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="27">
+    <cfRule type="expression" dxfId="108" priority="27">
       <formula>AND($B16&lt;&gt;1,$D16&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="56" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="107" priority="20" stopIfTrue="1">
       <formula>D13=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13:F13">
-    <cfRule type="expression" dxfId="55" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="106" priority="18" stopIfTrue="1">
       <formula>$B13=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="19">
+    <cfRule type="expression" dxfId="105" priority="19">
       <formula>$D13=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="21">
+    <cfRule type="expression" dxfId="104" priority="21">
       <formula>AND(B13&lt;&gt;1,D13=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="22">
+    <cfRule type="expression" dxfId="103" priority="22">
       <formula>AND($B13&lt;&gt;1,$D13&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9:F9">
-    <cfRule type="expression" dxfId="51" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="12" stopIfTrue="1">
       <formula>$B9=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="13">
+    <cfRule type="expression" dxfId="101" priority="13">
       <formula>$D9=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="15">
+    <cfRule type="expression" dxfId="100" priority="15">
       <formula>AND(C9&lt;&gt;1,E9=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="16">
+    <cfRule type="expression" dxfId="99" priority="16">
       <formula>AND($B9&lt;&gt;1,$D9&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="47" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="98" priority="8" stopIfTrue="1">
       <formula>D10=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:F10">
-    <cfRule type="expression" dxfId="46" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="6" stopIfTrue="1">
       <formula>$B10=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="7">
+    <cfRule type="expression" dxfId="96" priority="7">
       <formula>$D10=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="9">
+    <cfRule type="expression" dxfId="95" priority="9">
       <formula>AND(B10&lt;&gt;1,D10=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="10">
+    <cfRule type="expression" dxfId="94" priority="10">
       <formula>AND($B10&lt;&gt;1,$D10&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="42" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="3" stopIfTrue="1">
       <formula>D9=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="41" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="1" stopIfTrue="1">
       <formula>$B9=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="2">
+    <cfRule type="expression" dxfId="91" priority="2">
       <formula>$D9=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="4">
+    <cfRule type="expression" dxfId="90" priority="4">
       <formula>AND(B9&lt;&gt;1,D9=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="5">
+    <cfRule type="expression" dxfId="89" priority="5">
       <formula>AND($B9&lt;&gt;1,$D9&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3103,22 +3826,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D555DB45-06D3-4E53-8C52-4C0A4D00F5D5}">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="36"/>
-    <col min="2" max="2" width="26.5703125" style="36" customWidth="1"/>
-    <col min="3" max="3" width="56.35546875" style="36" customWidth="1"/>
-    <col min="4" max="4" width="25.0703125" style="36" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="36"/>
+    <col min="1" max="1" width="9.1796875" style="36"/>
+    <col min="2" max="2" width="26.54296875" style="36" customWidth="1"/>
+    <col min="3" max="3" width="56.36328125" style="36" customWidth="1"/>
+    <col min="4" max="4" width="25.08984375" style="36" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
         <v>21</v>
       </c>
@@ -3129,7 +3852,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="140.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="138" x14ac:dyDescent="0.25">
       <c r="A2" s="36">
         <v>1</v>
       </c>
@@ -3140,7 +3863,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="36">
         <v>2</v>
       </c>
@@ -3148,7 +3871,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="36">
         <v>4</v>
       </c>
@@ -3156,7 +3879,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="56" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A11" s="36">
         <v>5</v>
       </c>
@@ -3164,7 +3887,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="36">
         <v>6</v>
       </c>
@@ -3172,128 +3895,239 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="28" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A19" s="36">
         <v>7</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" s="36" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="126" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="124.2" x14ac:dyDescent="0.25">
       <c r="A22" s="36">
         <v>8</v>
       </c>
       <c r="B22" s="36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" s="36" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A25" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="36" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A28" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="36" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A30" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="36" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A34" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="36" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" s="36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="C38" s="40" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="55.2" x14ac:dyDescent="0.25">
+      <c r="A39" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="C39" s="36" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A42" s="36" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="B25" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" s="36" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="28" x14ac:dyDescent="0.3">
-      <c r="A28" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="B28" s="36" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="42" x14ac:dyDescent="0.3">
-      <c r="A30" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" s="36" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="28" x14ac:dyDescent="0.3">
-      <c r="A34" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="B34" s="36" t="s">
-        <v>58</v>
-      </c>
-      <c r="C34" s="36" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="C37" s="36" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="28" x14ac:dyDescent="0.3">
-      <c r="C38" s="40" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="56" x14ac:dyDescent="0.3">
-      <c r="A39" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="B39" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="C39" s="36" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="28" x14ac:dyDescent="0.3">
-      <c r="A42" s="36" t="s">
-        <v>67</v>
-      </c>
       <c r="B42" s="36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="36" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="36" t="s">
+      <c r="B45" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="B45" s="36" t="s">
+    </row>
+    <row r="47" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A47" s="36" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="28" x14ac:dyDescent="0.3">
-      <c r="A47" s="36" t="s">
+      <c r="B47" s="36" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="B47" s="36" t="s">
+      <c r="B49" s="36" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="36" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="B49" s="36" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="36" t="s">
-        <v>79</v>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C67"/>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C69"/>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="71" spans="3:3" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B88" s="50" t="s">
+        <v>97</v>
+      </c>
+      <c r="C88" s="48" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B89" s="51"/>
+      <c r="C89" s="48" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B90" s="51"/>
+      <c r="C90" s="48" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B91" s="51"/>
+      <c r="C91"/>
+    </row>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B92" s="51"/>
+      <c r="C92" s="48" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B93" s="51"/>
+      <c r="C93" s="48" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B94" s="52"/>
+      <c r="C94" s="49" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B88:B94"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="C38" r:id="rId1" xr:uid="{5C5B9DE7-052C-4C5F-828C-C463458523F2}"/>
   </hyperlinks>
@@ -3303,240 +4137,34 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C58DE228-9694-49AA-B7F0-62FF3C86A015}">
-  <dimension ref="A1:A19"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="82.78515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>92</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr codeName="TaskSetup">
-    <tabColor theme="6" tint="0.39997558519241921"/>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:O9"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="3.78515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="21" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" style="2" customWidth="1"/>
-    <col min="4" max="6" width="8.78515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="7.2109375" style="2" hidden="1" customWidth="1"/>
-    <col min="8" max="15" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="10.7109375" style="2" hidden="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:11" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="46" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="47" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="47"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-    </row>
-    <row r="2" spans="2:11" ht="83.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-    </row>
-    <row r="3" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-    </row>
-    <row r="4" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="5"/>
-    </row>
-    <row r="7" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="5"/>
-    </row>
-    <row r="8" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="5"/>
-      <c r="E8" s="25"/>
-    </row>
-    <row r="9" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="5"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:F1"/>
-  </mergeCells>
-  <phoneticPr fontId="27" type="noConversion"/>
-  <dataValidations count="4">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create an Assignment Setup in this worksheet. Insert or modify entries in Color Keys table starting in cell B4. Select cell G1 to navigate to To Do List. Tip is in cell B2" sqref="A1" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insert or modify Assigned To names in this column under this heading" sqref="B3" xr:uid="{00000000-0002-0000-0100-000002000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell, tip in cell below, and navigation link to To Do List worksheet in cell at right" sqref="B1" xr:uid="{00000000-0002-0000-0100-000003000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Navigation link to To Do List worksheet" sqref="E1 G1:K2" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
-  </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="G1:K2" location="'To Do List'!A1" tooltip="Select to navigate to To Do List worksheet" display="&lt; To Do List" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="E1:F1" location="'To Do List'!A1" tooltip="Click to navigate to To Do List worksheet" display="&lt; To Do List" xr:uid="{030E72E2-83DE-4827-9931-20D8B9FA68D2}"/>
-  </hyperlinks>
-  <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="65" fitToHeight="0" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69EEA948-B125-4EA3-895B-CADE82C01CA9}">
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q15"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.78515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="20.28515625" style="2" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" style="4" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="1.81640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="27.26953125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.7265625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="16.7265625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="18.54296875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="7.7265625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="20.26953125" style="2" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="17.26953125" style="4" hidden="1" customWidth="1"/>
     <col min="10" max="14" width="0" style="4" hidden="1" customWidth="1"/>
     <col min="15" max="17" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.7109375" style="2" hidden="1"/>
+    <col min="18" max="16384" width="10.7265625" style="2" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="66" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:17" ht="66" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -3559,11 +4187,11 @@
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
     </row>
-    <row r="2" spans="1:17" ht="21.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:17" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="12"/>
       <c r="B2" s="43">
         <f ca="1">TODAY()</f>
-        <v>44505</v>
+        <v>44598</v>
       </c>
       <c r="C2" s="43"/>
       <c r="D2" s="18"/>
@@ -3578,7 +4206,7 @@
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
     </row>
-    <row r="3" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="22" t="s">
         <v>9</v>
@@ -3599,7 +4227,7 @@
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
     </row>
-    <row r="4" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="22" t="s">
         <v>10</v>
@@ -3621,7 +4249,7 @@
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
     </row>
-    <row r="5" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="7"/>
       <c r="C5" s="14"/>
       <c r="D5" s="11"/>
@@ -3635,7 +4263,7 @@
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
     </row>
-    <row r="6" spans="1:17" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15"/>
       <c r="B6" s="24" t="s">
         <v>2</v>
@@ -3659,7 +4287,7 @@
       <c r="N6" s="15"/>
       <c r="O6" s="15"/>
     </row>
-    <row r="7" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="42" t="s">
         <v>12</v>
       </c>
@@ -3667,7 +4295,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="1"/>
@@ -3679,13 +4307,13 @@
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="42"/>
       <c r="B8" s="9">
         <v>0</v>
       </c>
       <c r="C8" s="41" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="1"/>
@@ -3697,7 +4325,7 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="42"/>
       <c r="B9" s="9">
         <v>0</v>
@@ -3715,12 +4343,12 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="9">
         <v>0</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="1"/>
@@ -3732,7 +4360,7 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="9"/>
       <c r="C11" s="8" t="s">
         <v>35</v>
@@ -3747,10 +4375,10 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="9"/>
       <c r="C12" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D12" s="30"/>
       <c r="E12" s="1"/>
@@ -3762,10 +4390,10 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="9"/>
       <c r="C13" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="1"/>
@@ -3777,7 +4405,7 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -3785,7 +4413,10 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>104</v>
+      </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -3793,98 +4424,118 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
     </row>
+    <row r="16" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="A7:A9"/>
   </mergeCells>
   <conditionalFormatting sqref="C11:C12 C9">
-    <cfRule type="expression" dxfId="29" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="33" stopIfTrue="1">
       <formula>D9=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:F12 D13:F13 D7:F9 C9">
-    <cfRule type="expression" dxfId="28" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="31" stopIfTrue="1">
       <formula>$B7=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="32">
+    <cfRule type="expression" dxfId="80" priority="32">
       <formula>$D7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="34">
+    <cfRule type="expression" dxfId="79" priority="34">
       <formula>AND(B7&lt;&gt;1,D7=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="35">
+    <cfRule type="expression" dxfId="78" priority="35">
       <formula>AND($B7&lt;&gt;1,$D7&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="expression" dxfId="24" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="28" stopIfTrue="1">
       <formula>D7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="expression" dxfId="23" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="26" stopIfTrue="1">
       <formula>$B7=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="27">
+    <cfRule type="expression" dxfId="75" priority="27">
       <formula>$D7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="29">
+    <cfRule type="expression" dxfId="74" priority="29">
       <formula>AND(B7&lt;&gt;1,D7=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="30">
+    <cfRule type="expression" dxfId="73" priority="30">
       <formula>AND($B7&lt;&gt;1,$D7&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="expression" dxfId="19" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="13" stopIfTrue="1">
       <formula>D8=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="expression" dxfId="18" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="11" stopIfTrue="1">
       <formula>$B8=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="12">
+    <cfRule type="expression" dxfId="70" priority="12">
       <formula>$D8=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="14">
+    <cfRule type="expression" dxfId="69" priority="14">
       <formula>AND(B8&lt;&gt;1,D8=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="15">
+    <cfRule type="expression" dxfId="68" priority="15">
       <formula>AND($B8&lt;&gt;1,$D8&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:F10">
-    <cfRule type="expression" dxfId="14" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="6" stopIfTrue="1">
       <formula>$B10=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="7">
+    <cfRule type="expression" dxfId="66" priority="7">
       <formula>$D10=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="8">
+    <cfRule type="expression" dxfId="65" priority="8">
       <formula>AND(C10&lt;&gt;1,E10=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="9">
+    <cfRule type="expression" dxfId="64" priority="9">
       <formula>AND($B10&lt;&gt;1,$D10&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="10" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="3" stopIfTrue="1">
       <formula>D10=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="9" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="1" stopIfTrue="1">
       <formula>$B10=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="2">
+    <cfRule type="expression" dxfId="61" priority="2">
       <formula>$D10=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="60" priority="4">
       <formula>AND(B10&lt;&gt;1,D10=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="59" priority="5">
       <formula>AND($B10&lt;&gt;1,$D10&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3967,7 +4618,873 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2B0A940-E58C-4F73-B098-D84B75D771FF}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.59999389629810485"/>
+    <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:Q17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="1.81640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="27.26953125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.7265625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="16.7265625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="18.54296875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="7.7265625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="20.26953125" style="2" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="17.26953125" style="4" hidden="1" customWidth="1"/>
+    <col min="10" max="14" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="15" max="17" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.7265625" style="2" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="66" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="19"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+    </row>
+    <row r="2" spans="1:17" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="12"/>
+      <c r="B2" s="43">
+        <f ca="1">TODAY()</f>
+        <v>44598</v>
+      </c>
+      <c r="C2" s="43"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+    </row>
+    <row r="3" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="23">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+    </row>
+    <row r="4" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="23">
+        <f ca="1">COUNTIFS(ToDoList4[Due Date],"&lt;"&amp;TODAY(),ToDoList4[Done],"&lt;&gt;1")</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+    </row>
+    <row r="5" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="7"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:17" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+      <c r="B6" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+    </row>
+    <row r="7" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="9">
+        <v>1</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="6">
+        <f ca="1">TODAY()-1</f>
+        <v>44597</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="42"/>
+      <c r="B8" s="9">
+        <v>1</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="6">
+        <f ca="1">TODAY()+2</f>
+        <v>44600</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="42"/>
+      <c r="B9" s="9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="6">
+        <f ca="1">TODAY()+1</f>
+        <v>44599</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="42"/>
+      <c r="B10" s="9">
+        <v>1</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="6">
+        <f ca="1">TODAY()+1</f>
+        <v>44599</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="42"/>
+      <c r="B11" s="9">
+        <v>1</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="6">
+        <f ca="1">TODAY()+2</f>
+        <v>44600</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="9">
+        <v>1</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="6">
+        <f ca="1">TODAY()+8</f>
+        <v>44606</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="32">
+        <v>1</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="34">
+        <f ca="1">TODAY()+5</f>
+        <v>44603</v>
+      </c>
+      <c r="E13" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="9"/>
+      <c r="C14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="6">
+        <f ca="1">TODAY()+2</f>
+        <v>44600</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="9"/>
+      <c r="C15" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="6">
+        <f ca="1">TODAY()+2</f>
+        <v>44600</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="9">
+        <v>1</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="6">
+        <f ca="1">TODAY()+3</f>
+        <v>44601</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="2:6" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="32">
+        <v>1</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="6">
+        <f ca="1">TODAY()+3</f>
+        <v>44601</v>
+      </c>
+      <c r="E17" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="39" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="A7:A11"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C7:C8 C14:C15 C11:C12">
+    <cfRule type="expression" dxfId="52" priority="48" stopIfTrue="1">
+      <formula>D7=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7:F8 C14:F15 C11:F12">
+    <cfRule type="expression" dxfId="51" priority="46" stopIfTrue="1">
+      <formula>$B7=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="50" priority="47">
+      <formula>$D7=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="49" priority="49">
+      <formula>AND(B7&lt;&gt;1,D7=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="48" priority="50">
+      <formula>AND($B7&lt;&gt;1,$D7&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16">
+    <cfRule type="expression" dxfId="47" priority="34" stopIfTrue="1">
+      <formula>D16=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F16">
+    <cfRule type="expression" dxfId="46" priority="41" stopIfTrue="1">
+      <formula>$B16=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="45" priority="42">
+      <formula>$D16=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="43">
+      <formula>AND(E16&lt;&gt;1,G16=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="43" priority="44">
+      <formula>AND($B16&lt;&gt;1,$D16&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16">
+    <cfRule type="expression" dxfId="42" priority="37" stopIfTrue="1">
+      <formula>$B16=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="41" priority="38">
+      <formula>$D16=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="39">
+      <formula>AND(C16&lt;&gt;1,E16=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="39" priority="40">
+      <formula>AND($B16&lt;&gt;1,$D16&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16">
+    <cfRule type="expression" dxfId="38" priority="32" stopIfTrue="1">
+      <formula>$B16=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="33">
+      <formula>$D16=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="35">
+      <formula>AND(B16&lt;&gt;1,D16=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="35" priority="36">
+      <formula>AND($B16&lt;&gt;1,$D16&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16">
+    <cfRule type="expression" dxfId="34" priority="28" stopIfTrue="1">
+      <formula>$B16=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="29">
+      <formula>$D16=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="30">
+      <formula>AND(D16&lt;&gt;1,F16=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="31" priority="31">
+      <formula>AND($B16&lt;&gt;1,$D16&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="expression" dxfId="30" priority="24" stopIfTrue="1">
+      <formula>D13=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13:F13">
+    <cfRule type="expression" dxfId="29" priority="22" stopIfTrue="1">
+      <formula>$B13=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="23">
+      <formula>$D13=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="25">
+      <formula>AND(B13&lt;&gt;1,D13=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="26">
+      <formula>AND($B13&lt;&gt;1,$D13&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9:F9">
+    <cfRule type="expression" dxfId="25" priority="17" stopIfTrue="1">
+      <formula>$B9=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="18">
+      <formula>$D9=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="23" priority="19">
+      <formula>AND(C9&lt;&gt;1,E9=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="20">
+      <formula>AND($B9&lt;&gt;1,$D9&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10">
+    <cfRule type="expression" dxfId="21" priority="13" stopIfTrue="1">
+      <formula>D10=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10:F10">
+    <cfRule type="expression" dxfId="20" priority="11" stopIfTrue="1">
+      <formula>$B10=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="12">
+      <formula>$D10=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="14">
+      <formula>AND(B10&lt;&gt;1,D10=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="15">
+      <formula>AND($B10&lt;&gt;1,$D10&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="expression" dxfId="16" priority="8" stopIfTrue="1">
+      <formula>D9=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="expression" dxfId="15" priority="6" stopIfTrue="1">
+      <formula>$B9=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="7">
+      <formula>$D9=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="9">
+      <formula>AND(B9&lt;&gt;1,D9=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="10">
+      <formula>AND($B9&lt;&gt;1,$D9&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17">
+    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
+      <formula>$B17=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>$D17=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>AND(C17&lt;&gt;1,E17=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="4">
+      <formula>AND($B17&lt;&gt;1,$D17&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="17">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select Assigned to names from the list. Select CANCEL, press ALT+DOWN ARROW for options, then DOWN ARROW and ENTER to make selection" sqref="F7:F17" xr:uid="{2FE444E8-B9F6-4A2B-BF95-B4C274A4F32D}">
+      <formula1>Assignedto</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select Priority from the list. Select CANCEL, press ALT+DOWN ARROW for options, then DOWN ARROW and ENTER to make selection" sqref="E7:E17" xr:uid="{3B7DA989-D9D7-45EB-A694-4BBC2A902FFB}">
+      <formula1>"High,Medium,Low"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="B5:C5" xr:uid="{C80793E2-BB46-4DF4-BC7C-50CAD9A525FB}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Overdue days are automatically updated in this cell. Enter details in table below. Table tip is in cell A6" sqref="C4" xr:uid="{8C640474-7820-4D3F-9B99-3124A4B62D1B}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Overdue days are automatically updated in cell at right" sqref="B4" xr:uid="{9FF29D43-B882-48D7-A5C6-895A87573A2F}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this C1. Date is automatically updated in cell B2, and Due Today and Overdue days in cell C3 and C4. Next tip is in cell below." sqref="B1" xr:uid="{C9E2F777-7448-4815-BC40-CF6E5F5D31C9}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell. Date is automatically updated in cell below, and Due Today and Overdue days in cell C3 and C4. Tip is in cell at right" sqref="C1" xr:uid="{0AFD76E5-F21C-4082-8C06-220E2A6042B6}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter value greater than 1 in this column under this heading to mark task as Done. Strikethrough formatting will automatically be applied" sqref="B6" xr:uid="{7EBE5C21-1ABC-48B2-910B-E213B3B96339}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select Assigned to names in this column under this heading. Press ALT+DOWN ARROW for options, then DOWN ARROW and ENTER to make selection" sqref="F6" xr:uid="{8A986117-9AC1-4C35-913B-286C57793C6C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select Priority in this column under this heading. Press ALT+DOWN ARROW for options, then DOWN ARROW and ENTER to make selection" sqref="E6" xr:uid="{11578A6A-BC58-4B58-927F-B2AD77DF2DFB}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Due Date in this column under this heading" sqref="D6" xr:uid="{08A06C66-56C5-48EA-8EB5-7241BF42BB9F}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Description in this column under this heading" sqref="C6" xr:uid="{8F8AA43C-4537-4612-8670-B809F8344078}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Due Today is automatically updated in this cell" sqref="C3" xr:uid="{67DB34A8-F864-473A-9365-C2BA853A7DB1}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Due Today is automatically updated in cell at right" sqref="B3" xr:uid="{64737FC3-EA72-4D82-9EB8-D15605E525AB}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Date is automatically updated in this cell and Due Today and Overdue days in cells below" sqref="B2:C2" xr:uid="{84A5C09C-FDE8-4D09-825F-238FFD61029F}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Navigation link to Assignment Setup worksheet" sqref="F1:G5" xr:uid="{F14332AA-C40D-42B2-8F6A-5CB94690F507}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create To Do List in this workbook. Enter details in To Do List table in this worksheet. Select cell F1 to navigate to Setup worksheet. Due &amp; Overdue days are automatically updated" sqref="A1" xr:uid="{660D059F-77C3-4234-920E-178B4B39853B}"/>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="F1" location="'Assignment Setup'!A1" tooltip="Click to navigate to TAssignment Setup" display="Setup &gt;" xr:uid="{4B637F1B-0B81-4292-B3A4-1E773EF0C176}"/>
+  </hyperlinks>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="58" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="51" id="{B865E691-8D2C-44A3-8FD3-18BE1230F257}">
+            <x14:iconSet iconSet="3Symbols2" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="formula">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>B7:B8 B14:B15 B11:B12</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="45" id="{1E829A64-0D67-48C9-AB6D-B403E2893716}">
+            <x14:iconSet iconSet="3Symbols2" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="formula">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>B16</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="27" id="{0D627A13-EEB7-4F63-AE4C-E8D1944F28AB}">
+            <x14:iconSet iconSet="3Symbols2" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="formula">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>B13</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="21" id="{964B918D-4811-482A-B0CF-38BB73069508}">
+            <x14:iconSet iconSet="3Symbols2" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="formula">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>B9</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="16" id="{933904E7-1814-4C90-9E7C-81BC06108A3B}">
+            <x14:iconSet iconSet="3Symbols2" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="formula">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>B10</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="5" id="{0F83DF3A-A6A3-4778-8500-28481AEDC69C}">
+            <x14:iconSet iconSet="3Symbols2" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="formula">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>B17</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="TaskSetup">
+    <tabColor theme="6" tint="0.39997558519241921"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:O9"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.81640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="21" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.26953125" style="2" customWidth="1"/>
+    <col min="4" max="6" width="8.81640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="7.1796875" style="2" hidden="1" customWidth="1"/>
+    <col min="8" max="15" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="16" max="16384" width="10.7265625" style="2" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="47"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+    </row>
+    <row r="2" spans="2:11" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+    </row>
+    <row r="3" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+    </row>
+    <row r="4" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="5"/>
+    </row>
+    <row r="7" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+    </row>
+    <row r="8" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="5"/>
+      <c r="E8" s="25"/>
+    </row>
+    <row r="9" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
+  <phoneticPr fontId="27" type="noConversion"/>
+  <dataValidations count="4">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create an Assignment Setup in this worksheet. Insert or modify entries in Color Keys table starting in cell B4. Select cell G1 to navigate to To Do List. Tip is in cell B2" sqref="A1" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insert or modify Assigned To names in this column under this heading" sqref="B3" xr:uid="{00000000-0002-0000-0100-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell, tip in cell below, and navigation link to To Do List worksheet in cell at right" sqref="B1" xr:uid="{00000000-0002-0000-0100-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Navigation link to To Do List worksheet" sqref="E1 G1:K2" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="G1:K2" location="'To Do List'!A1" tooltip="Select to navigate to To Do List worksheet" display="&lt; To Do List" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="E1:F1" location="'To Do List'!A1" tooltip="Click to navigate to To Do List worksheet" display="&lt; To Do List" xr:uid="{030E72E2-83DE-4827-9931-20D8B9FA68D2}"/>
+  </hyperlinks>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="65" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -3976,7 +5493,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DEEA25CC0A0AC24199CDC46C25B8B0BC" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e3b47856d4cf355c0dacb39e1084d14f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="6dc4bcd6-49db-4c07-9060-8acfc67cef9f" xmlns:ns3="fb0879af-3eba-417a-a55a-ffe6dcd6ca77" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a845a615265fdb1f7b12cc65ac20ecbd" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4184,16 +5701,17 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03CCC4C8-6A95-4999-B963-115A022CA31F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{920DC3BD-3C4B-4C78-91FF-63EB10F70D2C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -4201,7 +5719,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7118F064-9046-4DCB-A010-2D274D0FB549}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4219,14 +5737,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03CCC4C8-6A95-4999-B963-115A022CA31F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>